<commit_message>
Support for tax on interest from bank/bonds, refactored a lot of the tax code
</commit_message>
<xml_diff>
--- a/tests/Feature/config/cash_realistic.xlsx
+++ b/tests/Feature/config/cash_realistic.xlsx
@@ -3868,7 +3868,7 @@
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="1">
-        <v>0.0</v>
+        <v>220.0</v>
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="1">
@@ -3930,7 +3930,7 @@
       <c r="AG37" s="2"/>
       <c r="AH37" s="2"/>
       <c r="AI37" s="7">
-        <v>0.0</v>
+        <v>-220.0</v>
       </c>
       <c r="AJ37" s="1">
         <v>0</v>
@@ -3965,7 +3965,7 @@
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="1">
-        <v>0.0</v>
+        <v>667.0</v>
       </c>
       <c r="H38" s="2"/>
       <c r="I38" s="1">
@@ -4029,7 +4029,7 @@
       <c r="AG38" s="2"/>
       <c r="AH38" s="2"/>
       <c r="AI38" s="7">
-        <v>0.0</v>
+        <v>-667.0</v>
       </c>
       <c r="AJ38" s="1">
         <v>0</v>
@@ -4064,7 +4064,7 @@
       </c>
       <c r="F39" s="10"/>
       <c r="G39" s="9">
-        <v>0.0</v>
+        <v>915.0</v>
       </c>
       <c r="H39" s="10"/>
       <c r="I39" s="9">
@@ -4128,10 +4128,10 @@
       <c r="AG39" s="10"/>
       <c r="AH39" s="10"/>
       <c r="AI39" s="9">
-        <v>0.0</v>
+        <v>-915.0</v>
       </c>
       <c r="AJ39" s="9">
-        <v>0.0</v>
+        <v>-915.0</v>
       </c>
       <c r="AK39" s="10"/>
       <c r="AL39" s="9">
@@ -4163,7 +4163,7 @@
       </c>
       <c r="F40" s="14"/>
       <c r="G40" s="13">
-        <v>0.0</v>
+        <v>952.0</v>
       </c>
       <c r="H40" s="14"/>
       <c r="I40" s="13">
@@ -4227,10 +4227,10 @@
       <c r="AG40" s="14"/>
       <c r="AH40" s="14"/>
       <c r="AI40" s="13">
-        <v>0.0</v>
+        <v>-952.0</v>
       </c>
       <c r="AJ40" s="13">
-        <v>0.0</v>
+        <v>-1867.0</v>
       </c>
       <c r="AK40" s="14"/>
       <c r="AL40" s="13">
@@ -4262,7 +4262,7 @@
       </c>
       <c r="F41" s="2"/>
       <c r="G41" s="1">
-        <v>0.0</v>
+        <v>743.0</v>
       </c>
       <c r="H41" s="2"/>
       <c r="I41" s="1">
@@ -4326,10 +4326,10 @@
       <c r="AG41" s="2"/>
       <c r="AH41" s="2"/>
       <c r="AI41" s="7">
-        <v>0.0</v>
+        <v>-743.0</v>
       </c>
       <c r="AJ41" s="1">
-        <v>0.0</v>
+        <v>-2610.0</v>
       </c>
       <c r="AK41" s="2"/>
       <c r="AL41" s="1">
@@ -4361,7 +4361,7 @@
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="1">
-        <v>0.0</v>
+        <v>510.0</v>
       </c>
       <c r="H42" s="2"/>
       <c r="I42" s="1">
@@ -4425,10 +4425,10 @@
       <c r="AG42" s="2"/>
       <c r="AH42" s="2"/>
       <c r="AI42" s="7">
-        <v>0.0</v>
+        <v>-510.0</v>
       </c>
       <c r="AJ42" s="1">
-        <v>0.0</v>
+        <v>-3120.0</v>
       </c>
       <c r="AK42" s="2"/>
       <c r="AL42" s="1">
@@ -4460,7 +4460,7 @@
       </c>
       <c r="F43" s="2"/>
       <c r="G43" s="1">
-        <v>0.0</v>
+        <v>520.0</v>
       </c>
       <c r="H43" s="2"/>
       <c r="I43" s="1">
@@ -4524,10 +4524,10 @@
       <c r="AG43" s="2"/>
       <c r="AH43" s="2"/>
       <c r="AI43" s="7">
-        <v>0.0</v>
+        <v>-520.0</v>
       </c>
       <c r="AJ43" s="1">
-        <v>0.0</v>
+        <v>-3640.0</v>
       </c>
       <c r="AK43" s="2"/>
       <c r="AL43" s="1">
@@ -4559,7 +4559,7 @@
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="1">
-        <v>0.0</v>
+        <v>531.0</v>
       </c>
       <c r="H44" s="2"/>
       <c r="I44" s="1">
@@ -4623,10 +4623,10 @@
       <c r="AG44" s="2"/>
       <c r="AH44" s="2"/>
       <c r="AI44" s="7">
-        <v>0.0</v>
+        <v>-531.0</v>
       </c>
       <c r="AJ44" s="1">
-        <v>0.0</v>
+        <v>-4171.0</v>
       </c>
       <c r="AK44" s="2"/>
       <c r="AL44" s="1">
@@ -4658,7 +4658,7 @@
       </c>
       <c r="F45" s="2"/>
       <c r="G45" s="1">
-        <v>0.0</v>
+        <v>541.0</v>
       </c>
       <c r="H45" s="2"/>
       <c r="I45" s="1">
@@ -4722,10 +4722,10 @@
       <c r="AG45" s="2"/>
       <c r="AH45" s="2"/>
       <c r="AI45" s="7">
-        <v>0.0</v>
+        <v>-541.0</v>
       </c>
       <c r="AJ45" s="1">
-        <v>0.0</v>
+        <v>-4712.0</v>
       </c>
       <c r="AK45" s="2"/>
       <c r="AL45" s="1">
@@ -4757,7 +4757,7 @@
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="1">
-        <v>0.0</v>
+        <v>552.0</v>
       </c>
       <c r="H46" s="2"/>
       <c r="I46" s="1">
@@ -4821,10 +4821,10 @@
       <c r="AG46" s="2"/>
       <c r="AH46" s="2"/>
       <c r="AI46" s="7">
-        <v>0.0</v>
+        <v>-552.0</v>
       </c>
       <c r="AJ46" s="1">
-        <v>0.0</v>
+        <v>-5264.0</v>
       </c>
       <c r="AK46" s="2"/>
       <c r="AL46" s="1">
@@ -4856,7 +4856,7 @@
       </c>
       <c r="F47" s="2"/>
       <c r="G47" s="1">
-        <v>0.0</v>
+        <v>563.0</v>
       </c>
       <c r="H47" s="2"/>
       <c r="I47" s="1">
@@ -4920,10 +4920,10 @@
       <c r="AG47" s="2"/>
       <c r="AH47" s="2"/>
       <c r="AI47" s="7">
-        <v>0.0</v>
+        <v>-563.0</v>
       </c>
       <c r="AJ47" s="1">
-        <v>0.0</v>
+        <v>-5827.0</v>
       </c>
       <c r="AK47" s="2"/>
       <c r="AL47" s="1">
@@ -4955,7 +4955,7 @@
       </c>
       <c r="F48" s="2"/>
       <c r="G48" s="1">
-        <v>0.0</v>
+        <v>574.0</v>
       </c>
       <c r="H48" s="2"/>
       <c r="I48" s="1">
@@ -5019,10 +5019,10 @@
       <c r="AG48" s="2"/>
       <c r="AH48" s="2"/>
       <c r="AI48" s="7">
-        <v>0.0</v>
+        <v>-574.0</v>
       </c>
       <c r="AJ48" s="1">
-        <v>0.0</v>
+        <v>-6401.0</v>
       </c>
       <c r="AK48" s="2"/>
       <c r="AL48" s="1">
@@ -5054,7 +5054,7 @@
       </c>
       <c r="F49" s="2"/>
       <c r="G49" s="1">
-        <v>0.0</v>
+        <v>586.0</v>
       </c>
       <c r="H49" s="2"/>
       <c r="I49" s="1">
@@ -5118,10 +5118,10 @@
       <c r="AG49" s="2"/>
       <c r="AH49" s="2"/>
       <c r="AI49" s="7">
-        <v>0.0</v>
+        <v>-586.0</v>
       </c>
       <c r="AJ49" s="1">
-        <v>0.0</v>
+        <v>-6987.0</v>
       </c>
       <c r="AK49" s="2"/>
       <c r="AL49" s="1">
@@ -5153,7 +5153,7 @@
       </c>
       <c r="F50" s="2"/>
       <c r="G50" s="1">
-        <v>0.0</v>
+        <v>598.0</v>
       </c>
       <c r="H50" s="2"/>
       <c r="I50" s="1">
@@ -5217,10 +5217,10 @@
       <c r="AG50" s="2"/>
       <c r="AH50" s="2"/>
       <c r="AI50" s="7">
-        <v>0.0</v>
+        <v>-598.0</v>
       </c>
       <c r="AJ50" s="1">
-        <v>0.0</v>
+        <v>-7585.0</v>
       </c>
       <c r="AK50" s="2"/>
       <c r="AL50" s="1">
@@ -5252,7 +5252,7 @@
       </c>
       <c r="F51" s="2"/>
       <c r="G51" s="1">
-        <v>0.0</v>
+        <v>609.0</v>
       </c>
       <c r="H51" s="2"/>
       <c r="I51" s="1">
@@ -5316,10 +5316,10 @@
       <c r="AG51" s="2"/>
       <c r="AH51" s="2"/>
       <c r="AI51" s="7">
-        <v>0.0</v>
+        <v>-609.0</v>
       </c>
       <c r="AJ51" s="1">
-        <v>0.0</v>
+        <v>-8194.0</v>
       </c>
       <c r="AK51" s="2"/>
       <c r="AL51" s="1">
@@ -5351,7 +5351,7 @@
       </c>
       <c r="F52" s="2"/>
       <c r="G52" s="1">
-        <v>0.0</v>
+        <v>622.0</v>
       </c>
       <c r="H52" s="2"/>
       <c r="I52" s="1">
@@ -5415,10 +5415,10 @@
       <c r="AG52" s="2"/>
       <c r="AH52" s="2"/>
       <c r="AI52" s="7">
-        <v>0.0</v>
+        <v>-622.0</v>
       </c>
       <c r="AJ52" s="1">
-        <v>0.0</v>
+        <v>-8816.0</v>
       </c>
       <c r="AK52" s="2"/>
       <c r="AL52" s="1">
@@ -5450,7 +5450,7 @@
       </c>
       <c r="F53" s="17"/>
       <c r="G53" s="16">
-        <v>0.0</v>
+        <v>634.0</v>
       </c>
       <c r="H53" s="17"/>
       <c r="I53" s="16">
@@ -5514,10 +5514,10 @@
       <c r="AG53" s="17"/>
       <c r="AH53" s="17"/>
       <c r="AI53" s="16">
-        <v>0.0</v>
+        <v>-634.0</v>
       </c>
       <c r="AJ53" s="16">
-        <v>0.0</v>
+        <v>-9450.0</v>
       </c>
       <c r="AK53" s="17"/>
       <c r="AL53" s="16">
@@ -5549,7 +5549,7 @@
       </c>
       <c r="F54" s="2"/>
       <c r="G54" s="1">
-        <v>0.0</v>
+        <v>647.0</v>
       </c>
       <c r="H54" s="2"/>
       <c r="I54" s="1">
@@ -5613,10 +5613,10 @@
       <c r="AG54" s="2"/>
       <c r="AH54" s="2"/>
       <c r="AI54" s="7">
-        <v>0.0</v>
+        <v>-647.0</v>
       </c>
       <c r="AJ54" s="1">
-        <v>0.0</v>
+        <v>-10097.0</v>
       </c>
       <c r="AK54" s="2"/>
       <c r="AL54" s="1">
@@ -5648,7 +5648,7 @@
       </c>
       <c r="F55" s="2"/>
       <c r="G55" s="1">
-        <v>0.0</v>
+        <v>660.0</v>
       </c>
       <c r="H55" s="2"/>
       <c r="I55" s="1">
@@ -5712,10 +5712,10 @@
       <c r="AG55" s="2"/>
       <c r="AH55" s="2"/>
       <c r="AI55" s="7">
-        <v>0.0</v>
+        <v>-660.0</v>
       </c>
       <c r="AJ55" s="1">
-        <v>0.0</v>
+        <v>-10757.0</v>
       </c>
       <c r="AK55" s="2"/>
       <c r="AL55" s="1">
@@ -5747,7 +5747,7 @@
       </c>
       <c r="F56" s="2"/>
       <c r="G56" s="1">
-        <v>0.0</v>
+        <v>673.0</v>
       </c>
       <c r="H56" s="2"/>
       <c r="I56" s="1">
@@ -5811,10 +5811,10 @@
       <c r="AG56" s="2"/>
       <c r="AH56" s="2"/>
       <c r="AI56" s="7">
-        <v>0.0</v>
+        <v>-673.0</v>
       </c>
       <c r="AJ56" s="1">
-        <v>0.0</v>
+        <v>-11430.0</v>
       </c>
       <c r="AK56" s="2"/>
       <c r="AL56" s="1">
@@ -5846,7 +5846,7 @@
       </c>
       <c r="F57" s="17"/>
       <c r="G57" s="16">
-        <v>0.0</v>
+        <v>686.0</v>
       </c>
       <c r="H57" s="17"/>
       <c r="I57" s="16">
@@ -5910,10 +5910,10 @@
       <c r="AG57" s="17"/>
       <c r="AH57" s="17"/>
       <c r="AI57" s="16">
-        <v>0.0</v>
+        <v>-686.0</v>
       </c>
       <c r="AJ57" s="16">
-        <v>0.0</v>
+        <v>-12116.0</v>
       </c>
       <c r="AK57" s="17"/>
       <c r="AL57" s="16">
@@ -5945,7 +5945,7 @@
       </c>
       <c r="F58" s="2"/>
       <c r="G58" s="1">
-        <v>0.0</v>
+        <v>700.0</v>
       </c>
       <c r="H58" s="2"/>
       <c r="I58" s="1">
@@ -6009,10 +6009,10 @@
       <c r="AG58" s="2"/>
       <c r="AH58" s="2"/>
       <c r="AI58" s="7">
-        <v>0.0</v>
+        <v>-700.0</v>
       </c>
       <c r="AJ58" s="1">
-        <v>0.0</v>
+        <v>-12816.0</v>
       </c>
       <c r="AK58" s="2"/>
       <c r="AL58" s="1">
@@ -6044,7 +6044,7 @@
       </c>
       <c r="F59" s="2"/>
       <c r="G59" s="1">
-        <v>0.0</v>
+        <v>714.0</v>
       </c>
       <c r="H59" s="2"/>
       <c r="I59" s="1">
@@ -6108,10 +6108,10 @@
       <c r="AG59" s="2"/>
       <c r="AH59" s="2"/>
       <c r="AI59" s="7">
-        <v>0.0</v>
+        <v>-714.0</v>
       </c>
       <c r="AJ59" s="1">
-        <v>0.0</v>
+        <v>-13530.0</v>
       </c>
       <c r="AK59" s="2"/>
       <c r="AL59" s="1">
@@ -6143,7 +6143,7 @@
       </c>
       <c r="F60" s="2"/>
       <c r="G60" s="1">
-        <v>0.0</v>
+        <v>728.0</v>
       </c>
       <c r="H60" s="2"/>
       <c r="I60" s="1">
@@ -6207,10 +6207,10 @@
       <c r="AG60" s="2"/>
       <c r="AH60" s="2"/>
       <c r="AI60" s="7">
-        <v>0.0</v>
+        <v>-728.0</v>
       </c>
       <c r="AJ60" s="1">
-        <v>0.0</v>
+        <v>-14258.0</v>
       </c>
       <c r="AK60" s="2"/>
       <c r="AL60" s="1">
@@ -6242,7 +6242,7 @@
       </c>
       <c r="F61" s="2"/>
       <c r="G61" s="1">
-        <v>0.0</v>
+        <v>743.0</v>
       </c>
       <c r="H61" s="2"/>
       <c r="I61" s="1">
@@ -6306,10 +6306,10 @@
       <c r="AG61" s="2"/>
       <c r="AH61" s="2"/>
       <c r="AI61" s="7">
-        <v>0.0</v>
+        <v>-743.0</v>
       </c>
       <c r="AJ61" s="1">
-        <v>0.0</v>
+        <v>-15001.0</v>
       </c>
       <c r="AK61" s="2"/>
       <c r="AL61" s="1">
@@ -6341,7 +6341,7 @@
       </c>
       <c r="F62" s="2"/>
       <c r="G62" s="1">
-        <v>0.0</v>
+        <v>758.0</v>
       </c>
       <c r="H62" s="2"/>
       <c r="I62" s="1">
@@ -6405,10 +6405,10 @@
       <c r="AG62" s="2"/>
       <c r="AH62" s="2"/>
       <c r="AI62" s="7">
-        <v>0.0</v>
+        <v>-758.0</v>
       </c>
       <c r="AJ62" s="1">
-        <v>0.0</v>
+        <v>-15759.0</v>
       </c>
       <c r="AK62" s="2"/>
       <c r="AL62" s="1">
@@ -6440,7 +6440,7 @@
       </c>
       <c r="F63" s="2"/>
       <c r="G63" s="1">
-        <v>0.0</v>
+        <v>773.0</v>
       </c>
       <c r="H63" s="2"/>
       <c r="I63" s="1">
@@ -6504,10 +6504,10 @@
       <c r="AG63" s="2"/>
       <c r="AH63" s="2"/>
       <c r="AI63" s="7">
-        <v>0.0</v>
+        <v>-773.0</v>
       </c>
       <c r="AJ63" s="1">
-        <v>0.0</v>
+        <v>-16532.0</v>
       </c>
       <c r="AK63" s="2"/>
       <c r="AL63" s="1">
@@ -6539,7 +6539,7 @@
       </c>
       <c r="F64" s="2"/>
       <c r="G64" s="1">
-        <v>0.0</v>
+        <v>788.0</v>
       </c>
       <c r="H64" s="2"/>
       <c r="I64" s="1">
@@ -6603,10 +6603,10 @@
       <c r="AG64" s="2"/>
       <c r="AH64" s="2"/>
       <c r="AI64" s="7">
-        <v>0.0</v>
+        <v>-788.0</v>
       </c>
       <c r="AJ64" s="1">
-        <v>0.0</v>
+        <v>-17320.0</v>
       </c>
       <c r="AK64" s="2"/>
       <c r="AL64" s="1">
@@ -6638,7 +6638,7 @@
       </c>
       <c r="F65" s="2"/>
       <c r="G65" s="1">
-        <v>0.0</v>
+        <v>804.0</v>
       </c>
       <c r="H65" s="2"/>
       <c r="I65" s="1">
@@ -6702,10 +6702,10 @@
       <c r="AG65" s="2"/>
       <c r="AH65" s="2"/>
       <c r="AI65" s="7">
-        <v>0.0</v>
+        <v>-804.0</v>
       </c>
       <c r="AJ65" s="1">
-        <v>0.0</v>
+        <v>-18124.0</v>
       </c>
       <c r="AK65" s="2"/>
       <c r="AL65" s="1">
@@ -6737,7 +6737,7 @@
       </c>
       <c r="F66" s="2"/>
       <c r="G66" s="1">
-        <v>0.0</v>
+        <v>820.0</v>
       </c>
       <c r="H66" s="2"/>
       <c r="I66" s="1">
@@ -6801,10 +6801,10 @@
       <c r="AG66" s="2"/>
       <c r="AH66" s="2"/>
       <c r="AI66" s="7">
-        <v>0.0</v>
+        <v>-820.0</v>
       </c>
       <c r="AJ66" s="1">
-        <v>0.0</v>
+        <v>-18944.0</v>
       </c>
       <c r="AK66" s="2"/>
       <c r="AL66" s="1">
@@ -6836,7 +6836,7 @@
       </c>
       <c r="F67" s="2"/>
       <c r="G67" s="1">
-        <v>0.0</v>
+        <v>837.0</v>
       </c>
       <c r="H67" s="2"/>
       <c r="I67" s="1">
@@ -6900,10 +6900,10 @@
       <c r="AG67" s="2"/>
       <c r="AH67" s="2"/>
       <c r="AI67" s="7">
-        <v>0.0</v>
+        <v>-837.0</v>
       </c>
       <c r="AJ67" s="1">
-        <v>0.0</v>
+        <v>-19781.0</v>
       </c>
       <c r="AK67" s="2"/>
       <c r="AL67" s="1">
@@ -6935,7 +6935,7 @@
       </c>
       <c r="F68" s="2"/>
       <c r="G68" s="1">
-        <v>0.0</v>
+        <v>853.0</v>
       </c>
       <c r="H68" s="2"/>
       <c r="I68" s="1">
@@ -6999,10 +6999,10 @@
       <c r="AG68" s="2"/>
       <c r="AH68" s="2"/>
       <c r="AI68" s="7">
-        <v>0.0</v>
+        <v>-853.0</v>
       </c>
       <c r="AJ68" s="1">
-        <v>0.0</v>
+        <v>-20634.0</v>
       </c>
       <c r="AK68" s="2"/>
       <c r="AL68" s="1">
@@ -7034,7 +7034,7 @@
       </c>
       <c r="F69" s="2"/>
       <c r="G69" s="1">
-        <v>0.0</v>
+        <v>870.0</v>
       </c>
       <c r="H69" s="2"/>
       <c r="I69" s="1">
@@ -7098,10 +7098,10 @@
       <c r="AG69" s="2"/>
       <c r="AH69" s="2"/>
       <c r="AI69" s="7">
-        <v>0.0</v>
+        <v>-870.0</v>
       </c>
       <c r="AJ69" s="1">
-        <v>0.0</v>
+        <v>-21504.0</v>
       </c>
       <c r="AK69" s="2"/>
       <c r="AL69" s="1">
@@ -7133,7 +7133,7 @@
       </c>
       <c r="F70" s="2"/>
       <c r="G70" s="1">
-        <v>0.0</v>
+        <v>888.0</v>
       </c>
       <c r="H70" s="2"/>
       <c r="I70" s="1">
@@ -7197,10 +7197,10 @@
       <c r="AG70" s="2"/>
       <c r="AH70" s="2"/>
       <c r="AI70" s="7">
-        <v>0.0</v>
+        <v>-888.0</v>
       </c>
       <c r="AJ70" s="1">
-        <v>0.0</v>
+        <v>-22392.0</v>
       </c>
       <c r="AK70" s="2"/>
       <c r="AL70" s="1">
@@ -7232,7 +7232,7 @@
       </c>
       <c r="F71" s="2"/>
       <c r="G71" s="1">
-        <v>0.0</v>
+        <v>906.0</v>
       </c>
       <c r="H71" s="2"/>
       <c r="I71" s="1">
@@ -7296,10 +7296,10 @@
       <c r="AG71" s="2"/>
       <c r="AH71" s="2"/>
       <c r="AI71" s="7">
-        <v>0.0</v>
+        <v>-906.0</v>
       </c>
       <c r="AJ71" s="1">
-        <v>0.0</v>
+        <v>-23298.0</v>
       </c>
       <c r="AK71" s="2"/>
       <c r="AL71" s="1">
@@ -7331,7 +7331,7 @@
       </c>
       <c r="F72" s="20"/>
       <c r="G72" s="6">
-        <v>0.0</v>
+        <v>924.0</v>
       </c>
       <c r="H72" s="20"/>
       <c r="I72" s="6">
@@ -7395,10 +7395,10 @@
       <c r="AG72" s="20"/>
       <c r="AH72" s="20"/>
       <c r="AI72" s="6">
-        <v>0.0</v>
+        <v>-924.0</v>
       </c>
       <c r="AJ72" s="6">
-        <v>0.0</v>
+        <v>-24222.0</v>
       </c>
       <c r="AK72" s="20"/>
       <c r="AL72" s="6">
@@ -11057,7 +11057,7 @@
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="1">
-        <v>0.0</v>
+        <v>220.0</v>
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="1">
@@ -11119,7 +11119,7 @@
       <c r="AG37" s="2"/>
       <c r="AH37" s="2"/>
       <c r="AI37" s="7">
-        <v>0.0</v>
+        <v>-220.0</v>
       </c>
       <c r="AJ37" s="1">
         <v>0</v>
@@ -11154,7 +11154,7 @@
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="1">
-        <v>0.0</v>
+        <v>667.0</v>
       </c>
       <c r="H38" s="2"/>
       <c r="I38" s="1">
@@ -11218,7 +11218,7 @@
       <c r="AG38" s="2"/>
       <c r="AH38" s="2"/>
       <c r="AI38" s="7">
-        <v>0.0</v>
+        <v>-667.0</v>
       </c>
       <c r="AJ38" s="1">
         <v>0</v>
@@ -11253,7 +11253,7 @@
       </c>
       <c r="F39" s="10"/>
       <c r="G39" s="9">
-        <v>0.0</v>
+        <v>915.0</v>
       </c>
       <c r="H39" s="10"/>
       <c r="I39" s="9">
@@ -11317,10 +11317,10 @@
       <c r="AG39" s="10"/>
       <c r="AH39" s="10"/>
       <c r="AI39" s="9">
-        <v>0.0</v>
+        <v>-915.0</v>
       </c>
       <c r="AJ39" s="9">
-        <v>0.0</v>
+        <v>-915.0</v>
       </c>
       <c r="AK39" s="10"/>
       <c r="AL39" s="9">
@@ -11352,7 +11352,7 @@
       </c>
       <c r="F40" s="14"/>
       <c r="G40" s="13">
-        <v>0.0</v>
+        <v>952.0</v>
       </c>
       <c r="H40" s="14"/>
       <c r="I40" s="13">
@@ -11416,10 +11416,10 @@
       <c r="AG40" s="14"/>
       <c r="AH40" s="14"/>
       <c r="AI40" s="13">
-        <v>0.0</v>
+        <v>-952.0</v>
       </c>
       <c r="AJ40" s="13">
-        <v>0.0</v>
+        <v>-1867.0</v>
       </c>
       <c r="AK40" s="14"/>
       <c r="AL40" s="13">
@@ -11451,7 +11451,7 @@
       </c>
       <c r="F41" s="2"/>
       <c r="G41" s="1">
-        <v>0.0</v>
+        <v>743.0</v>
       </c>
       <c r="H41" s="2"/>
       <c r="I41" s="1">
@@ -11515,10 +11515,10 @@
       <c r="AG41" s="2"/>
       <c r="AH41" s="2"/>
       <c r="AI41" s="7">
-        <v>0.0</v>
+        <v>-743.0</v>
       </c>
       <c r="AJ41" s="1">
-        <v>0.0</v>
+        <v>-2610.0</v>
       </c>
       <c r="AK41" s="2"/>
       <c r="AL41" s="1">
@@ -11550,7 +11550,7 @@
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="1">
-        <v>0.0</v>
+        <v>510.0</v>
       </c>
       <c r="H42" s="2"/>
       <c r="I42" s="1">
@@ -11614,10 +11614,10 @@
       <c r="AG42" s="2"/>
       <c r="AH42" s="2"/>
       <c r="AI42" s="7">
-        <v>0.0</v>
+        <v>-510.0</v>
       </c>
       <c r="AJ42" s="1">
-        <v>0.0</v>
+        <v>-3120.0</v>
       </c>
       <c r="AK42" s="2"/>
       <c r="AL42" s="1">
@@ -11649,7 +11649,7 @@
       </c>
       <c r="F43" s="2"/>
       <c r="G43" s="1">
-        <v>0.0</v>
+        <v>520.0</v>
       </c>
       <c r="H43" s="2"/>
       <c r="I43" s="1">
@@ -11713,10 +11713,10 @@
       <c r="AG43" s="2"/>
       <c r="AH43" s="2"/>
       <c r="AI43" s="7">
-        <v>0.0</v>
+        <v>-520.0</v>
       </c>
       <c r="AJ43" s="1">
-        <v>0.0</v>
+        <v>-3640.0</v>
       </c>
       <c r="AK43" s="2"/>
       <c r="AL43" s="1">
@@ -11748,7 +11748,7 @@
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="1">
-        <v>0.0</v>
+        <v>531.0</v>
       </c>
       <c r="H44" s="2"/>
       <c r="I44" s="1">
@@ -11812,10 +11812,10 @@
       <c r="AG44" s="2"/>
       <c r="AH44" s="2"/>
       <c r="AI44" s="7">
-        <v>0.0</v>
+        <v>-531.0</v>
       </c>
       <c r="AJ44" s="1">
-        <v>0.0</v>
+        <v>-4171.0</v>
       </c>
       <c r="AK44" s="2"/>
       <c r="AL44" s="1">
@@ -11847,7 +11847,7 @@
       </c>
       <c r="F45" s="2"/>
       <c r="G45" s="1">
-        <v>0.0</v>
+        <v>541.0</v>
       </c>
       <c r="H45" s="2"/>
       <c r="I45" s="1">
@@ -11911,10 +11911,10 @@
       <c r="AG45" s="2"/>
       <c r="AH45" s="2"/>
       <c r="AI45" s="7">
-        <v>0.0</v>
+        <v>-541.0</v>
       </c>
       <c r="AJ45" s="1">
-        <v>0.0</v>
+        <v>-4712.0</v>
       </c>
       <c r="AK45" s="2"/>
       <c r="AL45" s="1">
@@ -11946,7 +11946,7 @@
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="1">
-        <v>0.0</v>
+        <v>552.0</v>
       </c>
       <c r="H46" s="2"/>
       <c r="I46" s="1">
@@ -12010,10 +12010,10 @@
       <c r="AG46" s="2"/>
       <c r="AH46" s="2"/>
       <c r="AI46" s="7">
-        <v>0.0</v>
+        <v>-552.0</v>
       </c>
       <c r="AJ46" s="1">
-        <v>0.0</v>
+        <v>-5264.0</v>
       </c>
       <c r="AK46" s="2"/>
       <c r="AL46" s="1">
@@ -12045,7 +12045,7 @@
       </c>
       <c r="F47" s="2"/>
       <c r="G47" s="1">
-        <v>0.0</v>
+        <v>563.0</v>
       </c>
       <c r="H47" s="2"/>
       <c r="I47" s="1">
@@ -12109,10 +12109,10 @@
       <c r="AG47" s="2"/>
       <c r="AH47" s="2"/>
       <c r="AI47" s="7">
-        <v>0.0</v>
+        <v>-563.0</v>
       </c>
       <c r="AJ47" s="1">
-        <v>0.0</v>
+        <v>-5827.0</v>
       </c>
       <c r="AK47" s="2"/>
       <c r="AL47" s="1">
@@ -12144,7 +12144,7 @@
       </c>
       <c r="F48" s="2"/>
       <c r="G48" s="1">
-        <v>0.0</v>
+        <v>574.0</v>
       </c>
       <c r="H48" s="2"/>
       <c r="I48" s="1">
@@ -12208,10 +12208,10 @@
       <c r="AG48" s="2"/>
       <c r="AH48" s="2"/>
       <c r="AI48" s="7">
-        <v>0.0</v>
+        <v>-574.0</v>
       </c>
       <c r="AJ48" s="1">
-        <v>0.0</v>
+        <v>-6401.0</v>
       </c>
       <c r="AK48" s="2"/>
       <c r="AL48" s="1">
@@ -12243,7 +12243,7 @@
       </c>
       <c r="F49" s="2"/>
       <c r="G49" s="1">
-        <v>0.0</v>
+        <v>586.0</v>
       </c>
       <c r="H49" s="2"/>
       <c r="I49" s="1">
@@ -12307,10 +12307,10 @@
       <c r="AG49" s="2"/>
       <c r="AH49" s="2"/>
       <c r="AI49" s="7">
-        <v>0.0</v>
+        <v>-586.0</v>
       </c>
       <c r="AJ49" s="1">
-        <v>0.0</v>
+        <v>-6987.0</v>
       </c>
       <c r="AK49" s="2"/>
       <c r="AL49" s="1">
@@ -12342,7 +12342,7 @@
       </c>
       <c r="F50" s="2"/>
       <c r="G50" s="1">
-        <v>0.0</v>
+        <v>598.0</v>
       </c>
       <c r="H50" s="2"/>
       <c r="I50" s="1">
@@ -12406,10 +12406,10 @@
       <c r="AG50" s="2"/>
       <c r="AH50" s="2"/>
       <c r="AI50" s="7">
-        <v>0.0</v>
+        <v>-598.0</v>
       </c>
       <c r="AJ50" s="1">
-        <v>0.0</v>
+        <v>-7585.0</v>
       </c>
       <c r="AK50" s="2"/>
       <c r="AL50" s="1">
@@ -12441,7 +12441,7 @@
       </c>
       <c r="F51" s="2"/>
       <c r="G51" s="1">
-        <v>0.0</v>
+        <v>609.0</v>
       </c>
       <c r="H51" s="2"/>
       <c r="I51" s="1">
@@ -12505,10 +12505,10 @@
       <c r="AG51" s="2"/>
       <c r="AH51" s="2"/>
       <c r="AI51" s="7">
-        <v>0.0</v>
+        <v>-609.0</v>
       </c>
       <c r="AJ51" s="1">
-        <v>0.0</v>
+        <v>-8194.0</v>
       </c>
       <c r="AK51" s="2"/>
       <c r="AL51" s="1">
@@ -12540,7 +12540,7 @@
       </c>
       <c r="F52" s="2"/>
       <c r="G52" s="1">
-        <v>0.0</v>
+        <v>622.0</v>
       </c>
       <c r="H52" s="2"/>
       <c r="I52" s="1">
@@ -12604,10 +12604,10 @@
       <c r="AG52" s="2"/>
       <c r="AH52" s="2"/>
       <c r="AI52" s="7">
-        <v>0.0</v>
+        <v>-622.0</v>
       </c>
       <c r="AJ52" s="1">
-        <v>0.0</v>
+        <v>-8816.0</v>
       </c>
       <c r="AK52" s="2"/>
       <c r="AL52" s="1">
@@ -12639,7 +12639,7 @@
       </c>
       <c r="F53" s="17"/>
       <c r="G53" s="16">
-        <v>0.0</v>
+        <v>634.0</v>
       </c>
       <c r="H53" s="17"/>
       <c r="I53" s="16">
@@ -12703,10 +12703,10 @@
       <c r="AG53" s="17"/>
       <c r="AH53" s="17"/>
       <c r="AI53" s="16">
-        <v>0.0</v>
+        <v>-634.0</v>
       </c>
       <c r="AJ53" s="16">
-        <v>0.0</v>
+        <v>-9450.0</v>
       </c>
       <c r="AK53" s="17"/>
       <c r="AL53" s="16">
@@ -12738,7 +12738,7 @@
       </c>
       <c r="F54" s="2"/>
       <c r="G54" s="1">
-        <v>0.0</v>
+        <v>647.0</v>
       </c>
       <c r="H54" s="2"/>
       <c r="I54" s="1">
@@ -12802,10 +12802,10 @@
       <c r="AG54" s="2"/>
       <c r="AH54" s="2"/>
       <c r="AI54" s="7">
-        <v>0.0</v>
+        <v>-647.0</v>
       </c>
       <c r="AJ54" s="1">
-        <v>0.0</v>
+        <v>-10097.0</v>
       </c>
       <c r="AK54" s="2"/>
       <c r="AL54" s="1">
@@ -12837,7 +12837,7 @@
       </c>
       <c r="F55" s="2"/>
       <c r="G55" s="1">
-        <v>0.0</v>
+        <v>660.0</v>
       </c>
       <c r="H55" s="2"/>
       <c r="I55" s="1">
@@ -12901,10 +12901,10 @@
       <c r="AG55" s="2"/>
       <c r="AH55" s="2"/>
       <c r="AI55" s="7">
-        <v>0.0</v>
+        <v>-660.0</v>
       </c>
       <c r="AJ55" s="1">
-        <v>0.0</v>
+        <v>-10757.0</v>
       </c>
       <c r="AK55" s="2"/>
       <c r="AL55" s="1">
@@ -12936,7 +12936,7 @@
       </c>
       <c r="F56" s="2"/>
       <c r="G56" s="1">
-        <v>0.0</v>
+        <v>673.0</v>
       </c>
       <c r="H56" s="2"/>
       <c r="I56" s="1">
@@ -13000,10 +13000,10 @@
       <c r="AG56" s="2"/>
       <c r="AH56" s="2"/>
       <c r="AI56" s="7">
-        <v>0.0</v>
+        <v>-673.0</v>
       </c>
       <c r="AJ56" s="1">
-        <v>0.0</v>
+        <v>-11430.0</v>
       </c>
       <c r="AK56" s="2"/>
       <c r="AL56" s="1">
@@ -13035,7 +13035,7 @@
       </c>
       <c r="F57" s="17"/>
       <c r="G57" s="16">
-        <v>0.0</v>
+        <v>686.0</v>
       </c>
       <c r="H57" s="17"/>
       <c r="I57" s="16">
@@ -13099,10 +13099,10 @@
       <c r="AG57" s="17"/>
       <c r="AH57" s="17"/>
       <c r="AI57" s="16">
-        <v>0.0</v>
+        <v>-686.0</v>
       </c>
       <c r="AJ57" s="16">
-        <v>0.0</v>
+        <v>-12116.0</v>
       </c>
       <c r="AK57" s="17"/>
       <c r="AL57" s="16">
@@ -13134,7 +13134,7 @@
       </c>
       <c r="F58" s="2"/>
       <c r="G58" s="1">
-        <v>0.0</v>
+        <v>700.0</v>
       </c>
       <c r="H58" s="2"/>
       <c r="I58" s="1">
@@ -13198,10 +13198,10 @@
       <c r="AG58" s="2"/>
       <c r="AH58" s="2"/>
       <c r="AI58" s="7">
-        <v>0.0</v>
+        <v>-700.0</v>
       </c>
       <c r="AJ58" s="1">
-        <v>0.0</v>
+        <v>-12816.0</v>
       </c>
       <c r="AK58" s="2"/>
       <c r="AL58" s="1">
@@ -13233,7 +13233,7 @@
       </c>
       <c r="F59" s="2"/>
       <c r="G59" s="1">
-        <v>0.0</v>
+        <v>714.0</v>
       </c>
       <c r="H59" s="2"/>
       <c r="I59" s="1">
@@ -13297,10 +13297,10 @@
       <c r="AG59" s="2"/>
       <c r="AH59" s="2"/>
       <c r="AI59" s="7">
-        <v>0.0</v>
+        <v>-714.0</v>
       </c>
       <c r="AJ59" s="1">
-        <v>0.0</v>
+        <v>-13530.0</v>
       </c>
       <c r="AK59" s="2"/>
       <c r="AL59" s="1">
@@ -13332,7 +13332,7 @@
       </c>
       <c r="F60" s="2"/>
       <c r="G60" s="1">
-        <v>0.0</v>
+        <v>728.0</v>
       </c>
       <c r="H60" s="2"/>
       <c r="I60" s="1">
@@ -13396,10 +13396,10 @@
       <c r="AG60" s="2"/>
       <c r="AH60" s="2"/>
       <c r="AI60" s="7">
-        <v>0.0</v>
+        <v>-728.0</v>
       </c>
       <c r="AJ60" s="1">
-        <v>0.0</v>
+        <v>-14258.0</v>
       </c>
       <c r="AK60" s="2"/>
       <c r="AL60" s="1">
@@ -13431,7 +13431,7 @@
       </c>
       <c r="F61" s="2"/>
       <c r="G61" s="1">
-        <v>0.0</v>
+        <v>743.0</v>
       </c>
       <c r="H61" s="2"/>
       <c r="I61" s="1">
@@ -13495,10 +13495,10 @@
       <c r="AG61" s="2"/>
       <c r="AH61" s="2"/>
       <c r="AI61" s="7">
-        <v>0.0</v>
+        <v>-743.0</v>
       </c>
       <c r="AJ61" s="1">
-        <v>0.0</v>
+        <v>-15001.0</v>
       </c>
       <c r="AK61" s="2"/>
       <c r="AL61" s="1">
@@ -13530,7 +13530,7 @@
       </c>
       <c r="F62" s="2"/>
       <c r="G62" s="1">
-        <v>0.0</v>
+        <v>758.0</v>
       </c>
       <c r="H62" s="2"/>
       <c r="I62" s="1">
@@ -13594,10 +13594,10 @@
       <c r="AG62" s="2"/>
       <c r="AH62" s="2"/>
       <c r="AI62" s="7">
-        <v>0.0</v>
+        <v>-758.0</v>
       </c>
       <c r="AJ62" s="1">
-        <v>0.0</v>
+        <v>-15759.0</v>
       </c>
       <c r="AK62" s="2"/>
       <c r="AL62" s="1">
@@ -13629,7 +13629,7 @@
       </c>
       <c r="F63" s="2"/>
       <c r="G63" s="1">
-        <v>0.0</v>
+        <v>773.0</v>
       </c>
       <c r="H63" s="2"/>
       <c r="I63" s="1">
@@ -13693,10 +13693,10 @@
       <c r="AG63" s="2"/>
       <c r="AH63" s="2"/>
       <c r="AI63" s="7">
-        <v>0.0</v>
+        <v>-773.0</v>
       </c>
       <c r="AJ63" s="1">
-        <v>0.0</v>
+        <v>-16532.0</v>
       </c>
       <c r="AK63" s="2"/>
       <c r="AL63" s="1">
@@ -13728,7 +13728,7 @@
       </c>
       <c r="F64" s="2"/>
       <c r="G64" s="1">
-        <v>0.0</v>
+        <v>788.0</v>
       </c>
       <c r="H64" s="2"/>
       <c r="I64" s="1">
@@ -13792,10 +13792,10 @@
       <c r="AG64" s="2"/>
       <c r="AH64" s="2"/>
       <c r="AI64" s="7">
-        <v>0.0</v>
+        <v>-788.0</v>
       </c>
       <c r="AJ64" s="1">
-        <v>0.0</v>
+        <v>-17320.0</v>
       </c>
       <c r="AK64" s="2"/>
       <c r="AL64" s="1">
@@ -13827,7 +13827,7 @@
       </c>
       <c r="F65" s="2"/>
       <c r="G65" s="1">
-        <v>0.0</v>
+        <v>804.0</v>
       </c>
       <c r="H65" s="2"/>
       <c r="I65" s="1">
@@ -13891,10 +13891,10 @@
       <c r="AG65" s="2"/>
       <c r="AH65" s="2"/>
       <c r="AI65" s="7">
-        <v>0.0</v>
+        <v>-804.0</v>
       </c>
       <c r="AJ65" s="1">
-        <v>0.0</v>
+        <v>-18124.0</v>
       </c>
       <c r="AK65" s="2"/>
       <c r="AL65" s="1">
@@ -13926,7 +13926,7 @@
       </c>
       <c r="F66" s="2"/>
       <c r="G66" s="1">
-        <v>0.0</v>
+        <v>820.0</v>
       </c>
       <c r="H66" s="2"/>
       <c r="I66" s="1">
@@ -13990,10 +13990,10 @@
       <c r="AG66" s="2"/>
       <c r="AH66" s="2"/>
       <c r="AI66" s="7">
-        <v>0.0</v>
+        <v>-820.0</v>
       </c>
       <c r="AJ66" s="1">
-        <v>0.0</v>
+        <v>-18944.0</v>
       </c>
       <c r="AK66" s="2"/>
       <c r="AL66" s="1">
@@ -14025,7 +14025,7 @@
       </c>
       <c r="F67" s="2"/>
       <c r="G67" s="1">
-        <v>0.0</v>
+        <v>837.0</v>
       </c>
       <c r="H67" s="2"/>
       <c r="I67" s="1">
@@ -14089,10 +14089,10 @@
       <c r="AG67" s="2"/>
       <c r="AH67" s="2"/>
       <c r="AI67" s="7">
-        <v>0.0</v>
+        <v>-837.0</v>
       </c>
       <c r="AJ67" s="1">
-        <v>0.0</v>
+        <v>-19781.0</v>
       </c>
       <c r="AK67" s="2"/>
       <c r="AL67" s="1">
@@ -14124,7 +14124,7 @@
       </c>
       <c r="F68" s="2"/>
       <c r="G68" s="1">
-        <v>0.0</v>
+        <v>853.0</v>
       </c>
       <c r="H68" s="2"/>
       <c r="I68" s="1">
@@ -14188,10 +14188,10 @@
       <c r="AG68" s="2"/>
       <c r="AH68" s="2"/>
       <c r="AI68" s="7">
-        <v>0.0</v>
+        <v>-853.0</v>
       </c>
       <c r="AJ68" s="1">
-        <v>0.0</v>
+        <v>-20634.0</v>
       </c>
       <c r="AK68" s="2"/>
       <c r="AL68" s="1">
@@ -14223,7 +14223,7 @@
       </c>
       <c r="F69" s="2"/>
       <c r="G69" s="1">
-        <v>0.0</v>
+        <v>870.0</v>
       </c>
       <c r="H69" s="2"/>
       <c r="I69" s="1">
@@ -14287,10 +14287,10 @@
       <c r="AG69" s="2"/>
       <c r="AH69" s="2"/>
       <c r="AI69" s="7">
-        <v>0.0</v>
+        <v>-870.0</v>
       </c>
       <c r="AJ69" s="1">
-        <v>0.0</v>
+        <v>-21504.0</v>
       </c>
       <c r="AK69" s="2"/>
       <c r="AL69" s="1">
@@ -14322,7 +14322,7 @@
       </c>
       <c r="F70" s="2"/>
       <c r="G70" s="1">
-        <v>0.0</v>
+        <v>888.0</v>
       </c>
       <c r="H70" s="2"/>
       <c r="I70" s="1">
@@ -14386,10 +14386,10 @@
       <c r="AG70" s="2"/>
       <c r="AH70" s="2"/>
       <c r="AI70" s="7">
-        <v>0.0</v>
+        <v>-888.0</v>
       </c>
       <c r="AJ70" s="1">
-        <v>0.0</v>
+        <v>-22392.0</v>
       </c>
       <c r="AK70" s="2"/>
       <c r="AL70" s="1">
@@ -14421,7 +14421,7 @@
       </c>
       <c r="F71" s="2"/>
       <c r="G71" s="1">
-        <v>0.0</v>
+        <v>906.0</v>
       </c>
       <c r="H71" s="2"/>
       <c r="I71" s="1">
@@ -14485,10 +14485,10 @@
       <c r="AG71" s="2"/>
       <c r="AH71" s="2"/>
       <c r="AI71" s="7">
-        <v>0.0</v>
+        <v>-906.0</v>
       </c>
       <c r="AJ71" s="1">
-        <v>0.0</v>
+        <v>-23298.0</v>
       </c>
       <c r="AK71" s="2"/>
       <c r="AL71" s="1">
@@ -14520,7 +14520,7 @@
       </c>
       <c r="F72" s="20"/>
       <c r="G72" s="6">
-        <v>0.0</v>
+        <v>924.0</v>
       </c>
       <c r="H72" s="20"/>
       <c r="I72" s="6">
@@ -14584,10 +14584,10 @@
       <c r="AG72" s="20"/>
       <c r="AH72" s="20"/>
       <c r="AI72" s="6">
-        <v>0.0</v>
+        <v>-924.0</v>
       </c>
       <c r="AJ72" s="6">
-        <v>0.0</v>
+        <v>-24222.0</v>
       </c>
       <c r="AK72" s="20"/>
       <c r="AL72" s="6">
@@ -21681,9 +21681,11 @@
       <c r="E37" s="6"/>
       <c r="F37" s="2"/>
       <c r="G37" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H37" s="2"/>
+        <v>220.0</v>
+      </c>
+      <c r="H37" s="2">
+        <v>0.22</v>
+      </c>
       <c r="I37" s="1"/>
       <c r="J37" s="2"/>
       <c r="K37" s="1"/>
@@ -21735,7 +21737,7 @@
       <c r="AG37" s="2"/>
       <c r="AH37" s="2"/>
       <c r="AI37" s="7">
-        <v>0.0</v>
+        <v>-220.0</v>
       </c>
       <c r="AJ37" s="1"/>
       <c r="AK37" s="2"/>
@@ -21768,9 +21770,11 @@
       <c r="E38" s="6"/>
       <c r="F38" s="2"/>
       <c r="G38" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H38" s="2"/>
+        <v>667.0</v>
+      </c>
+      <c r="H38" s="2">
+        <v>0.22</v>
+      </c>
       <c r="I38" s="1"/>
       <c r="J38" s="2"/>
       <c r="K38" s="1"/>
@@ -21822,7 +21826,7 @@
       <c r="AG38" s="2"/>
       <c r="AH38" s="2"/>
       <c r="AI38" s="7">
-        <v>0.0</v>
+        <v>-667.0</v>
       </c>
       <c r="AJ38" s="1"/>
       <c r="AK38" s="2"/>
@@ -21853,9 +21857,11 @@
       <c r="E39" s="9"/>
       <c r="F39" s="10"/>
       <c r="G39" s="9">
-        <v>0.0</v>
-      </c>
-      <c r="H39" s="10"/>
+        <v>915.0</v>
+      </c>
+      <c r="H39" s="10">
+        <v>0.22</v>
+      </c>
       <c r="I39" s="9"/>
       <c r="J39" s="10"/>
       <c r="K39" s="9"/>
@@ -21907,10 +21913,10 @@
       <c r="AG39" s="10"/>
       <c r="AH39" s="10"/>
       <c r="AI39" s="9">
-        <v>0.0</v>
+        <v>-915.0</v>
       </c>
       <c r="AJ39" s="9">
-        <v>0.0</v>
+        <v>-915.0</v>
       </c>
       <c r="AK39" s="10"/>
       <c r="AL39" s="9">
@@ -21940,9 +21946,11 @@
       <c r="E40" s="13"/>
       <c r="F40" s="14"/>
       <c r="G40" s="13">
-        <v>0.0</v>
-      </c>
-      <c r="H40" s="14"/>
+        <v>952.0</v>
+      </c>
+      <c r="H40" s="14">
+        <v>0.22</v>
+      </c>
       <c r="I40" s="13"/>
       <c r="J40" s="14"/>
       <c r="K40" s="13"/>
@@ -21994,10 +22002,10 @@
       <c r="AG40" s="14"/>
       <c r="AH40" s="14"/>
       <c r="AI40" s="13">
-        <v>0.0</v>
+        <v>-952.0</v>
       </c>
       <c r="AJ40" s="13">
-        <v>0.0</v>
+        <v>-1867.0</v>
       </c>
       <c r="AK40" s="14"/>
       <c r="AL40" s="13">
@@ -22027,9 +22035,11 @@
       <c r="E41" s="6"/>
       <c r="F41" s="2"/>
       <c r="G41" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H41" s="2"/>
+        <v>743.0</v>
+      </c>
+      <c r="H41" s="2">
+        <v>0.22</v>
+      </c>
       <c r="I41" s="1"/>
       <c r="J41" s="2"/>
       <c r="K41" s="1"/>
@@ -22081,10 +22091,10 @@
       <c r="AG41" s="2"/>
       <c r="AH41" s="2"/>
       <c r="AI41" s="7">
-        <v>0.0</v>
+        <v>-743.0</v>
       </c>
       <c r="AJ41" s="1">
-        <v>0.0</v>
+        <v>-2610.0</v>
       </c>
       <c r="AK41" s="2"/>
       <c r="AL41" s="1">
@@ -22114,9 +22124,11 @@
       <c r="E42" s="6"/>
       <c r="F42" s="2"/>
       <c r="G42" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H42" s="2"/>
+        <v>510.0</v>
+      </c>
+      <c r="H42" s="2">
+        <v>0.22</v>
+      </c>
       <c r="I42" s="1"/>
       <c r="J42" s="2"/>
       <c r="K42" s="1"/>
@@ -22168,10 +22180,10 @@
       <c r="AG42" s="2"/>
       <c r="AH42" s="2"/>
       <c r="AI42" s="7">
-        <v>0.0</v>
+        <v>-510.0</v>
       </c>
       <c r="AJ42" s="1">
-        <v>0.0</v>
+        <v>-3120.0</v>
       </c>
       <c r="AK42" s="2"/>
       <c r="AL42" s="1">
@@ -22201,9 +22213,11 @@
       <c r="E43" s="6"/>
       <c r="F43" s="2"/>
       <c r="G43" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H43" s="2"/>
+        <v>520.0</v>
+      </c>
+      <c r="H43" s="2">
+        <v>0.22</v>
+      </c>
       <c r="I43" s="1"/>
       <c r="J43" s="2"/>
       <c r="K43" s="1"/>
@@ -22255,10 +22269,10 @@
       <c r="AG43" s="2"/>
       <c r="AH43" s="2"/>
       <c r="AI43" s="7">
-        <v>0.0</v>
+        <v>-520.0</v>
       </c>
       <c r="AJ43" s="1">
-        <v>0.0</v>
+        <v>-3640.0</v>
       </c>
       <c r="AK43" s="2"/>
       <c r="AL43" s="1">
@@ -22288,9 +22302,11 @@
       <c r="E44" s="6"/>
       <c r="F44" s="2"/>
       <c r="G44" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H44" s="2"/>
+        <v>531.0</v>
+      </c>
+      <c r="H44" s="2">
+        <v>0.22</v>
+      </c>
       <c r="I44" s="1"/>
       <c r="J44" s="2"/>
       <c r="K44" s="1"/>
@@ -22342,10 +22358,10 @@
       <c r="AG44" s="2"/>
       <c r="AH44" s="2"/>
       <c r="AI44" s="7">
-        <v>0.0</v>
+        <v>-531.0</v>
       </c>
       <c r="AJ44" s="1">
-        <v>0.0</v>
+        <v>-4171.0</v>
       </c>
       <c r="AK44" s="2"/>
       <c r="AL44" s="1">
@@ -22375,9 +22391,11 @@
       <c r="E45" s="6"/>
       <c r="F45" s="2"/>
       <c r="G45" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H45" s="2"/>
+        <v>541.0</v>
+      </c>
+      <c r="H45" s="2">
+        <v>0.22</v>
+      </c>
       <c r="I45" s="1"/>
       <c r="J45" s="2"/>
       <c r="K45" s="1"/>
@@ -22429,10 +22447,10 @@
       <c r="AG45" s="2"/>
       <c r="AH45" s="2"/>
       <c r="AI45" s="7">
-        <v>0.0</v>
+        <v>-541.0</v>
       </c>
       <c r="AJ45" s="1">
-        <v>0.0</v>
+        <v>-4712.0</v>
       </c>
       <c r="AK45" s="2"/>
       <c r="AL45" s="1">
@@ -22462,9 +22480,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="2"/>
       <c r="G46" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H46" s="2"/>
+        <v>552.0</v>
+      </c>
+      <c r="H46" s="2">
+        <v>0.22</v>
+      </c>
       <c r="I46" s="1"/>
       <c r="J46" s="2"/>
       <c r="K46" s="1"/>
@@ -22516,10 +22536,10 @@
       <c r="AG46" s="2"/>
       <c r="AH46" s="2"/>
       <c r="AI46" s="7">
-        <v>0.0</v>
+        <v>-552.0</v>
       </c>
       <c r="AJ46" s="1">
-        <v>0.0</v>
+        <v>-5264.0</v>
       </c>
       <c r="AK46" s="2"/>
       <c r="AL46" s="1">
@@ -22549,9 +22569,11 @@
       <c r="E47" s="6"/>
       <c r="F47" s="2"/>
       <c r="G47" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H47" s="2"/>
+        <v>563.0</v>
+      </c>
+      <c r="H47" s="2">
+        <v>0.22</v>
+      </c>
       <c r="I47" s="1"/>
       <c r="J47" s="2"/>
       <c r="K47" s="1"/>
@@ -22603,10 +22625,10 @@
       <c r="AG47" s="2"/>
       <c r="AH47" s="2"/>
       <c r="AI47" s="7">
-        <v>0.0</v>
+        <v>-563.0</v>
       </c>
       <c r="AJ47" s="1">
-        <v>0.0</v>
+        <v>-5827.0</v>
       </c>
       <c r="AK47" s="2"/>
       <c r="AL47" s="1">
@@ -22636,9 +22658,11 @@
       <c r="E48" s="6"/>
       <c r="F48" s="2"/>
       <c r="G48" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H48" s="2"/>
+        <v>574.0</v>
+      </c>
+      <c r="H48" s="2">
+        <v>0.22</v>
+      </c>
       <c r="I48" s="1"/>
       <c r="J48" s="2"/>
       <c r="K48" s="1"/>
@@ -22690,10 +22714,10 @@
       <c r="AG48" s="2"/>
       <c r="AH48" s="2"/>
       <c r="AI48" s="7">
-        <v>0.0</v>
+        <v>-574.0</v>
       </c>
       <c r="AJ48" s="1">
-        <v>0.0</v>
+        <v>-6401.0</v>
       </c>
       <c r="AK48" s="2"/>
       <c r="AL48" s="1">
@@ -22723,9 +22747,11 @@
       <c r="E49" s="6"/>
       <c r="F49" s="2"/>
       <c r="G49" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H49" s="2"/>
+        <v>586.0</v>
+      </c>
+      <c r="H49" s="2">
+        <v>0.22</v>
+      </c>
       <c r="I49" s="1"/>
       <c r="J49" s="2"/>
       <c r="K49" s="1"/>
@@ -22777,10 +22803,10 @@
       <c r="AG49" s="2"/>
       <c r="AH49" s="2"/>
       <c r="AI49" s="7">
-        <v>0.0</v>
+        <v>-586.0</v>
       </c>
       <c r="AJ49" s="1">
-        <v>0.0</v>
+        <v>-6987.0</v>
       </c>
       <c r="AK49" s="2"/>
       <c r="AL49" s="1">
@@ -22810,9 +22836,11 @@
       <c r="E50" s="6"/>
       <c r="F50" s="2"/>
       <c r="G50" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H50" s="2"/>
+        <v>598.0</v>
+      </c>
+      <c r="H50" s="2">
+        <v>0.22</v>
+      </c>
       <c r="I50" s="1"/>
       <c r="J50" s="2"/>
       <c r="K50" s="1"/>
@@ -22864,10 +22892,10 @@
       <c r="AG50" s="2"/>
       <c r="AH50" s="2"/>
       <c r="AI50" s="7">
-        <v>0.0</v>
+        <v>-598.0</v>
       </c>
       <c r="AJ50" s="1">
-        <v>0.0</v>
+        <v>-7585.0</v>
       </c>
       <c r="AK50" s="2"/>
       <c r="AL50" s="1">
@@ -22897,9 +22925,11 @@
       <c r="E51" s="6"/>
       <c r="F51" s="2"/>
       <c r="G51" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H51" s="2"/>
+        <v>609.0</v>
+      </c>
+      <c r="H51" s="2">
+        <v>0.22</v>
+      </c>
       <c r="I51" s="1"/>
       <c r="J51" s="2"/>
       <c r="K51" s="1"/>
@@ -22951,10 +22981,10 @@
       <c r="AG51" s="2"/>
       <c r="AH51" s="2"/>
       <c r="AI51" s="7">
-        <v>0.0</v>
+        <v>-609.0</v>
       </c>
       <c r="AJ51" s="1">
-        <v>0.0</v>
+        <v>-8194.0</v>
       </c>
       <c r="AK51" s="2"/>
       <c r="AL51" s="1">
@@ -22984,9 +23014,11 @@
       <c r="E52" s="6"/>
       <c r="F52" s="2"/>
       <c r="G52" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H52" s="2"/>
+        <v>622.0</v>
+      </c>
+      <c r="H52" s="2">
+        <v>0.22</v>
+      </c>
       <c r="I52" s="1"/>
       <c r="J52" s="2"/>
       <c r="K52" s="1"/>
@@ -23038,10 +23070,10 @@
       <c r="AG52" s="2"/>
       <c r="AH52" s="2"/>
       <c r="AI52" s="7">
-        <v>0.0</v>
+        <v>-622.0</v>
       </c>
       <c r="AJ52" s="1">
-        <v>0.0</v>
+        <v>-8816.0</v>
       </c>
       <c r="AK52" s="2"/>
       <c r="AL52" s="1">
@@ -23071,9 +23103,11 @@
       <c r="E53" s="16"/>
       <c r="F53" s="17"/>
       <c r="G53" s="16">
-        <v>0.0</v>
-      </c>
-      <c r="H53" s="17"/>
+        <v>634.0</v>
+      </c>
+      <c r="H53" s="17">
+        <v>0.22</v>
+      </c>
       <c r="I53" s="16"/>
       <c r="J53" s="17"/>
       <c r="K53" s="16"/>
@@ -23125,10 +23159,10 @@
       <c r="AG53" s="17"/>
       <c r="AH53" s="17"/>
       <c r="AI53" s="16">
-        <v>0.0</v>
+        <v>-634.0</v>
       </c>
       <c r="AJ53" s="16">
-        <v>0.0</v>
+        <v>-9450.0</v>
       </c>
       <c r="AK53" s="17"/>
       <c r="AL53" s="16">
@@ -23158,9 +23192,11 @@
       <c r="E54" s="6"/>
       <c r="F54" s="2"/>
       <c r="G54" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H54" s="2"/>
+        <v>647.0</v>
+      </c>
+      <c r="H54" s="2">
+        <v>0.22</v>
+      </c>
       <c r="I54" s="1"/>
       <c r="J54" s="2"/>
       <c r="K54" s="1"/>
@@ -23212,10 +23248,10 @@
       <c r="AG54" s="2"/>
       <c r="AH54" s="2"/>
       <c r="AI54" s="7">
-        <v>0.0</v>
+        <v>-647.0</v>
       </c>
       <c r="AJ54" s="1">
-        <v>0.0</v>
+        <v>-10097.0</v>
       </c>
       <c r="AK54" s="2"/>
       <c r="AL54" s="1">
@@ -23245,9 +23281,11 @@
       <c r="E55" s="6"/>
       <c r="F55" s="2"/>
       <c r="G55" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H55" s="2"/>
+        <v>660.0</v>
+      </c>
+      <c r="H55" s="2">
+        <v>0.22</v>
+      </c>
       <c r="I55" s="1"/>
       <c r="J55" s="2"/>
       <c r="K55" s="1"/>
@@ -23299,10 +23337,10 @@
       <c r="AG55" s="2"/>
       <c r="AH55" s="2"/>
       <c r="AI55" s="7">
-        <v>0.0</v>
+        <v>-660.0</v>
       </c>
       <c r="AJ55" s="1">
-        <v>0.0</v>
+        <v>-10757.0</v>
       </c>
       <c r="AK55" s="2"/>
       <c r="AL55" s="1">
@@ -23332,9 +23370,11 @@
       <c r="E56" s="6"/>
       <c r="F56" s="2"/>
       <c r="G56" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H56" s="2"/>
+        <v>673.0</v>
+      </c>
+      <c r="H56" s="2">
+        <v>0.22</v>
+      </c>
       <c r="I56" s="1"/>
       <c r="J56" s="2"/>
       <c r="K56" s="1"/>
@@ -23386,10 +23426,10 @@
       <c r="AG56" s="2"/>
       <c r="AH56" s="2"/>
       <c r="AI56" s="7">
-        <v>0.0</v>
+        <v>-673.0</v>
       </c>
       <c r="AJ56" s="1">
-        <v>0.0</v>
+        <v>-11430.0</v>
       </c>
       <c r="AK56" s="2"/>
       <c r="AL56" s="1">
@@ -23419,9 +23459,11 @@
       <c r="E57" s="16"/>
       <c r="F57" s="17"/>
       <c r="G57" s="16">
-        <v>0.0</v>
-      </c>
-      <c r="H57" s="17"/>
+        <v>686.0</v>
+      </c>
+      <c r="H57" s="17">
+        <v>0.22</v>
+      </c>
       <c r="I57" s="16"/>
       <c r="J57" s="17"/>
       <c r="K57" s="16"/>
@@ -23473,10 +23515,10 @@
       <c r="AG57" s="17"/>
       <c r="AH57" s="17"/>
       <c r="AI57" s="16">
-        <v>0.0</v>
+        <v>-686.0</v>
       </c>
       <c r="AJ57" s="16">
-        <v>0.0</v>
+        <v>-12116.0</v>
       </c>
       <c r="AK57" s="17"/>
       <c r="AL57" s="16">
@@ -23506,9 +23548,11 @@
       <c r="E58" s="6"/>
       <c r="F58" s="2"/>
       <c r="G58" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H58" s="2"/>
+        <v>700.0</v>
+      </c>
+      <c r="H58" s="2">
+        <v>0.22</v>
+      </c>
       <c r="I58" s="1"/>
       <c r="J58" s="2"/>
       <c r="K58" s="1"/>
@@ -23560,10 +23604,10 @@
       <c r="AG58" s="2"/>
       <c r="AH58" s="2"/>
       <c r="AI58" s="7">
-        <v>0.0</v>
+        <v>-700.0</v>
       </c>
       <c r="AJ58" s="1">
-        <v>0.0</v>
+        <v>-12816.0</v>
       </c>
       <c r="AK58" s="2"/>
       <c r="AL58" s="1">
@@ -23593,9 +23637,11 @@
       <c r="E59" s="6"/>
       <c r="F59" s="2"/>
       <c r="G59" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H59" s="2"/>
+        <v>714.0</v>
+      </c>
+      <c r="H59" s="2">
+        <v>0.22</v>
+      </c>
       <c r="I59" s="1"/>
       <c r="J59" s="2"/>
       <c r="K59" s="1"/>
@@ -23647,10 +23693,10 @@
       <c r="AG59" s="2"/>
       <c r="AH59" s="2"/>
       <c r="AI59" s="7">
-        <v>0.0</v>
+        <v>-714.0</v>
       </c>
       <c r="AJ59" s="1">
-        <v>0.0</v>
+        <v>-13530.0</v>
       </c>
       <c r="AK59" s="2"/>
       <c r="AL59" s="1">
@@ -23680,9 +23726,11 @@
       <c r="E60" s="6"/>
       <c r="F60" s="2"/>
       <c r="G60" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H60" s="2"/>
+        <v>728.0</v>
+      </c>
+      <c r="H60" s="2">
+        <v>0.22</v>
+      </c>
       <c r="I60" s="1"/>
       <c r="J60" s="2"/>
       <c r="K60" s="1"/>
@@ -23734,10 +23782,10 @@
       <c r="AG60" s="2"/>
       <c r="AH60" s="2"/>
       <c r="AI60" s="7">
-        <v>0.0</v>
+        <v>-728.0</v>
       </c>
       <c r="AJ60" s="1">
-        <v>0.0</v>
+        <v>-14258.0</v>
       </c>
       <c r="AK60" s="2"/>
       <c r="AL60" s="1">
@@ -23767,9 +23815,11 @@
       <c r="E61" s="6"/>
       <c r="F61" s="2"/>
       <c r="G61" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H61" s="2"/>
+        <v>743.0</v>
+      </c>
+      <c r="H61" s="2">
+        <v>0.22</v>
+      </c>
       <c r="I61" s="1"/>
       <c r="J61" s="2"/>
       <c r="K61" s="1"/>
@@ -23821,10 +23871,10 @@
       <c r="AG61" s="2"/>
       <c r="AH61" s="2"/>
       <c r="AI61" s="7">
-        <v>0.0</v>
+        <v>-743.0</v>
       </c>
       <c r="AJ61" s="1">
-        <v>0.0</v>
+        <v>-15001.0</v>
       </c>
       <c r="AK61" s="2"/>
       <c r="AL61" s="1">
@@ -23854,9 +23904,11 @@
       <c r="E62" s="6"/>
       <c r="F62" s="2"/>
       <c r="G62" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H62" s="2"/>
+        <v>758.0</v>
+      </c>
+      <c r="H62" s="2">
+        <v>0.22</v>
+      </c>
       <c r="I62" s="1"/>
       <c r="J62" s="2"/>
       <c r="K62" s="1"/>
@@ -23908,10 +23960,10 @@
       <c r="AG62" s="2"/>
       <c r="AH62" s="2"/>
       <c r="AI62" s="7">
-        <v>0.0</v>
+        <v>-758.0</v>
       </c>
       <c r="AJ62" s="1">
-        <v>0.0</v>
+        <v>-15759.0</v>
       </c>
       <c r="AK62" s="2"/>
       <c r="AL62" s="1">
@@ -23941,9 +23993,11 @@
       <c r="E63" s="6"/>
       <c r="F63" s="2"/>
       <c r="G63" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H63" s="2"/>
+        <v>773.0</v>
+      </c>
+      <c r="H63" s="2">
+        <v>0.22</v>
+      </c>
       <c r="I63" s="1"/>
       <c r="J63" s="2"/>
       <c r="K63" s="1"/>
@@ -23995,10 +24049,10 @@
       <c r="AG63" s="2"/>
       <c r="AH63" s="2"/>
       <c r="AI63" s="7">
-        <v>0.0</v>
+        <v>-773.0</v>
       </c>
       <c r="AJ63" s="1">
-        <v>0.0</v>
+        <v>-16532.0</v>
       </c>
       <c r="AK63" s="2"/>
       <c r="AL63" s="1">
@@ -24028,9 +24082,11 @@
       <c r="E64" s="6"/>
       <c r="F64" s="2"/>
       <c r="G64" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H64" s="2"/>
+        <v>788.0</v>
+      </c>
+      <c r="H64" s="2">
+        <v>0.22</v>
+      </c>
       <c r="I64" s="1"/>
       <c r="J64" s="2"/>
       <c r="K64" s="1"/>
@@ -24082,10 +24138,10 @@
       <c r="AG64" s="2"/>
       <c r="AH64" s="2"/>
       <c r="AI64" s="7">
-        <v>0.0</v>
+        <v>-788.0</v>
       </c>
       <c r="AJ64" s="1">
-        <v>0.0</v>
+        <v>-17320.0</v>
       </c>
       <c r="AK64" s="2"/>
       <c r="AL64" s="1">
@@ -24115,9 +24171,11 @@
       <c r="E65" s="6"/>
       <c r="F65" s="2"/>
       <c r="G65" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H65" s="2"/>
+        <v>804.0</v>
+      </c>
+      <c r="H65" s="2">
+        <v>0.22</v>
+      </c>
       <c r="I65" s="1"/>
       <c r="J65" s="2"/>
       <c r="K65" s="1"/>
@@ -24169,10 +24227,10 @@
       <c r="AG65" s="2"/>
       <c r="AH65" s="2"/>
       <c r="AI65" s="7">
-        <v>0.0</v>
+        <v>-804.0</v>
       </c>
       <c r="AJ65" s="1">
-        <v>0.0</v>
+        <v>-18124.0</v>
       </c>
       <c r="AK65" s="2"/>
       <c r="AL65" s="1">
@@ -24202,9 +24260,11 @@
       <c r="E66" s="6"/>
       <c r="F66" s="2"/>
       <c r="G66" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H66" s="2"/>
+        <v>820.0</v>
+      </c>
+      <c r="H66" s="2">
+        <v>0.22</v>
+      </c>
       <c r="I66" s="1"/>
       <c r="J66" s="2"/>
       <c r="K66" s="1"/>
@@ -24256,10 +24316,10 @@
       <c r="AG66" s="2"/>
       <c r="AH66" s="2"/>
       <c r="AI66" s="7">
-        <v>0.0</v>
+        <v>-820.0</v>
       </c>
       <c r="AJ66" s="1">
-        <v>0.0</v>
+        <v>-18944.0</v>
       </c>
       <c r="AK66" s="2"/>
       <c r="AL66" s="1">
@@ -24289,9 +24349,11 @@
       <c r="E67" s="6"/>
       <c r="F67" s="2"/>
       <c r="G67" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H67" s="2"/>
+        <v>837.0</v>
+      </c>
+      <c r="H67" s="2">
+        <v>0.22</v>
+      </c>
       <c r="I67" s="1"/>
       <c r="J67" s="2"/>
       <c r="K67" s="1"/>
@@ -24343,10 +24405,10 @@
       <c r="AG67" s="2"/>
       <c r="AH67" s="2"/>
       <c r="AI67" s="7">
-        <v>0.0</v>
+        <v>-837.0</v>
       </c>
       <c r="AJ67" s="1">
-        <v>0.0</v>
+        <v>-19781.0</v>
       </c>
       <c r="AK67" s="2"/>
       <c r="AL67" s="1">
@@ -24376,9 +24438,11 @@
       <c r="E68" s="6"/>
       <c r="F68" s="2"/>
       <c r="G68" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H68" s="2"/>
+        <v>853.0</v>
+      </c>
+      <c r="H68" s="2">
+        <v>0.22</v>
+      </c>
       <c r="I68" s="1"/>
       <c r="J68" s="2"/>
       <c r="K68" s="1"/>
@@ -24430,10 +24494,10 @@
       <c r="AG68" s="2"/>
       <c r="AH68" s="2"/>
       <c r="AI68" s="7">
-        <v>0.0</v>
+        <v>-853.0</v>
       </c>
       <c r="AJ68" s="1">
-        <v>0.0</v>
+        <v>-20634.0</v>
       </c>
       <c r="AK68" s="2"/>
       <c r="AL68" s="1">
@@ -24463,9 +24527,11 @@
       <c r="E69" s="6"/>
       <c r="F69" s="2"/>
       <c r="G69" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H69" s="2"/>
+        <v>870.0</v>
+      </c>
+      <c r="H69" s="2">
+        <v>0.22</v>
+      </c>
       <c r="I69" s="1"/>
       <c r="J69" s="2"/>
       <c r="K69" s="1"/>
@@ -24517,10 +24583,10 @@
       <c r="AG69" s="2"/>
       <c r="AH69" s="2"/>
       <c r="AI69" s="7">
-        <v>0.0</v>
+        <v>-870.0</v>
       </c>
       <c r="AJ69" s="1">
-        <v>0.0</v>
+        <v>-21504.0</v>
       </c>
       <c r="AK69" s="2"/>
       <c r="AL69" s="1">
@@ -24550,9 +24616,11 @@
       <c r="E70" s="6"/>
       <c r="F70" s="2"/>
       <c r="G70" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H70" s="2"/>
+        <v>888.0</v>
+      </c>
+      <c r="H70" s="2">
+        <v>0.22</v>
+      </c>
       <c r="I70" s="1"/>
       <c r="J70" s="2"/>
       <c r="K70" s="1"/>
@@ -24604,10 +24672,10 @@
       <c r="AG70" s="2"/>
       <c r="AH70" s="2"/>
       <c r="AI70" s="7">
-        <v>0.0</v>
+        <v>-888.0</v>
       </c>
       <c r="AJ70" s="1">
-        <v>0.0</v>
+        <v>-22392.0</v>
       </c>
       <c r="AK70" s="2"/>
       <c r="AL70" s="1">
@@ -24637,9 +24705,11 @@
       <c r="E71" s="6"/>
       <c r="F71" s="2"/>
       <c r="G71" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="H71" s="2"/>
+        <v>906.0</v>
+      </c>
+      <c r="H71" s="2">
+        <v>0.22</v>
+      </c>
       <c r="I71" s="1"/>
       <c r="J71" s="2"/>
       <c r="K71" s="1"/>
@@ -24691,10 +24761,10 @@
       <c r="AG71" s="2"/>
       <c r="AH71" s="2"/>
       <c r="AI71" s="7">
-        <v>0.0</v>
+        <v>-906.0</v>
       </c>
       <c r="AJ71" s="1">
-        <v>0.0</v>
+        <v>-23298.0</v>
       </c>
       <c r="AK71" s="2"/>
       <c r="AL71" s="1">
@@ -24724,9 +24794,11 @@
       <c r="E72" s="6"/>
       <c r="F72" s="20"/>
       <c r="G72" s="6">
-        <v>0.0</v>
-      </c>
-      <c r="H72" s="20"/>
+        <v>924.0</v>
+      </c>
+      <c r="H72" s="20">
+        <v>0.22</v>
+      </c>
       <c r="I72" s="6"/>
       <c r="J72" s="20"/>
       <c r="K72" s="6"/>
@@ -24778,10 +24850,10 @@
       <c r="AG72" s="20"/>
       <c r="AH72" s="20"/>
       <c r="AI72" s="6">
-        <v>0.0</v>
+        <v>-924.0</v>
       </c>
       <c r="AJ72" s="6">
-        <v>0.0</v>
+        <v>-24222.0</v>
       </c>
       <c r="AK72" s="20"/>
       <c r="AL72" s="6">

</xml_diff>